<commit_message>
Commit: start of the set params function
</commit_message>
<xml_diff>
--- a/Support Data/BC survival.xlsx
+++ b/Support Data/BC survival.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cm1om\Documents\Research\Cancer\Bladder\Bladder_cancer_model\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cm1om\Documents\Research\Cancer\Bladder\Bladder_cancer_model\Support Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98C60F46-AF3C-4884-9735-05CD5D604315}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7300950F-6C66-4B49-8F95-3C348F3CF176}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{CEB37473-6591-494F-9B0C-E97D5E01BB77}"/>
   </bookViews>
@@ -1924,7 +1924,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6D40557-BB4B-40BD-B462-28670AE2DA58}">
   <dimension ref="A1:AI288"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
+    <sheetView topLeftCell="L19" workbookViewId="0">
       <selection activeCell="N1" sqref="N1:Y1"/>
     </sheetView>
   </sheetViews>
@@ -14544,7 +14544,7 @@
   <dimension ref="A1:N48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16284,7 +16284,7 @@
         <f>Sheet1!X42</f>
         <v>20.055698924731182</v>
       </c>
-      <c r="J38">
+      <c r="J38" s="23">
         <f>Sheet1!Y42</f>
         <v>12.977127975626095</v>
       </c>
@@ -16766,7 +16766,7 @@
   <dimension ref="A1:O37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="A31" sqref="A31:XFD31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17658,16 +17658,13 @@
         <v>61.794329334787349</v>
       </c>
       <c r="M16" s="23">
-        <f t="shared" si="0"/>
-        <v>15.024371323327285</v>
+        <v>13.968837209302325</v>
       </c>
       <c r="N16" s="23">
-        <f t="shared" si="0"/>
-        <v>9.7306471456692911</v>
+        <v>10.262344160104988</v>
       </c>
       <c r="O16" s="23">
-        <f t="shared" si="0"/>
-        <v>21.980430107526878</v>
+        <v>20.055698924731182</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
@@ -17717,16 +17714,13 @@
         <v>59.9</v>
       </c>
       <c r="M17" s="23">
-        <f>mortality!G38</f>
-        <v>13.968837209302325</v>
+        <v>14.2</v>
       </c>
       <c r="N17" s="23">
-        <f>mortality!H38</f>
-        <v>10.262344160104988</v>
+        <v>10.4</v>
       </c>
       <c r="O17" s="23">
-        <f>mortality!I38</f>
-        <v>20.055698924731182</v>
+        <v>17.899999999999999</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
@@ -17776,16 +17770,13 @@
         <v>53.7</v>
       </c>
       <c r="M18" s="23">
-        <f>mortality!G39</f>
-        <v>14.2</v>
+        <v>15.4</v>
       </c>
       <c r="N18" s="23">
-        <f>mortality!H39</f>
-        <v>10.4</v>
+        <v>12.9</v>
       </c>
       <c r="O18" s="23">
-        <f>mortality!I39</f>
-        <v>17.899999999999999</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
@@ -18295,16 +18286,16 @@
         <v>55.457748908029544</v>
       </c>
       <c r="M27" s="23">
-        <f t="shared" si="1"/>
-        <v>14.468394520928936</v>
+        <f>mortality!J38</f>
+        <v>12.977127975626095</v>
       </c>
       <c r="N27" s="23">
-        <f t="shared" si="1"/>
-        <v>10.763609499247792</v>
+        <f>mortality!K38</f>
+        <v>8.8082477303817939</v>
       </c>
       <c r="O27" s="23">
-        <f t="shared" si="1"/>
-        <v>14.255653220486472</v>
+        <f>mortality!L38</f>
+        <v>15.207244773244835</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
@@ -18354,16 +18345,13 @@
         <v>56.081946768992111</v>
       </c>
       <c r="M28" s="23">
-        <f t="shared" si="1"/>
-        <v>15.0925923818915</v>
+        <v>12.977127975626095</v>
       </c>
       <c r="N28" s="23">
-        <f t="shared" si="1"/>
-        <v>11.387807360210356</v>
+        <v>8.8082477303817939</v>
       </c>
       <c r="O28" s="23">
-        <f t="shared" si="1"/>
-        <v>14.879851081449036</v>
+        <v>15.207244773244835</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
@@ -18413,16 +18401,13 @@
         <v>51.571657754010687</v>
       </c>
       <c r="M29" s="23">
-        <f>mortality!J38</f>
-        <v>12.977127975626095</v>
+        <v>12.225668449197858</v>
       </c>
       <c r="N29" s="23">
-        <f>mortality!K38</f>
-        <v>8.8082477303817939</v>
+        <v>8.954010695187165</v>
       </c>
       <c r="O29" s="23">
-        <f>mortality!L38</f>
-        <v>15.207244773244835</v>
+        <v>15.411229946524061</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
@@ -18460,28 +18445,22 @@
         <v>49.160962566844916</v>
       </c>
       <c r="J30" s="23">
-        <f>mortality!J28</f>
-        <v>41.326203208556144</v>
+        <v>27.378609625668446</v>
       </c>
       <c r="K30" s="23">
-        <f>mortality!K28</f>
-        <v>36.504812834224595</v>
+        <v>22.815508021390372</v>
       </c>
       <c r="L30" s="23">
-        <f>mortality!L28</f>
-        <v>46.233689839572186</v>
+        <v>31.94171122994652</v>
       </c>
       <c r="M30" s="23">
-        <f>mortality!J39</f>
-        <v>12.225668449197858</v>
+        <v>13.258823529411764</v>
       </c>
       <c r="N30" s="23">
-        <f>mortality!K39</f>
-        <v>8.954010695187165</v>
+        <v>11.106417112299464</v>
       </c>
       <c r="O30" s="23">
-        <f>mortality!L39</f>
-        <v>15.411229946524061</v>
+        <v>15.497326203208555</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
@@ -18696,16 +18675,13 @@
         <v>47.289609416328716</v>
       </c>
       <c r="M34" s="23">
-        <f>mortality!J42</f>
-        <v>9.6560363258588993</v>
+        <v>9.0512741342602165</v>
       </c>
       <c r="N34" s="23">
-        <f>mortality!K42</f>
-        <v>7.0720266048544032</v>
+        <v>6.1435677447200749</v>
       </c>
       <c r="O34" s="23">
-        <f>mortality!L42</f>
-        <v>9.5076537381553319</v>
+        <v>10.606733749406061</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
@@ -18814,16 +18790,13 @@
         <v>22.71028037383179</v>
       </c>
       <c r="M36" s="23">
-        <f>mortality!J44</f>
-        <v>8.5271469015413626</v>
+        <v>9.247750865051902</v>
       </c>
       <c r="N36" s="23">
-        <f>mortality!K44</f>
-        <v>6.2452343504246608</v>
+        <v>7.7464926077382827</v>
       </c>
       <c r="O36" s="23">
-        <f>mortality!L44</f>
-        <v>10.749009122365523</v>
+        <v>10.809059452658069</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>